<commit_message>
implementing person view, fixing memory leaks, fixing code bugs
</commit_message>
<xml_diff>
--- a/data/import_template_dep_dropdowns_with_sample_v2 - Αντιγραφή.xlsx
+++ b/data/import_template_dep_dropdowns_with_sample_v2 - Αντιγραφή.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\group8\Documents\DEV\ai-e-nis\mil-tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E23554-73CA-429F-9559-A9EE8E052F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC30394B-F2AD-4FC8-AEA0-890EB8AA2969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="780" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="780" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="1" state="hidden" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="353">
   <si>
     <t>OrganizationType</t>
   </si>
@@ -872,9 +872,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>parent</t>
-  </si>
-  <si>
     <t>ΠΖ</t>
   </si>
   <si>
@@ -1152,6 +1149,12 @@
   </si>
   <si>
     <t>Θέμα 2</t>
+  </si>
+  <si>
+    <t>Στήλη1</t>
+  </si>
+  <si>
+    <t>organizationImage</t>
   </si>
 </sst>
 </file>
@@ -1408,14 +1411,15 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="T_Organizations" displayName="T_Organizations" ref="A1:E401">
-  <autoFilter ref="A1:E401" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="T_Organizations" displayName="T_Organizations" ref="A1:F401">
+  <autoFilter ref="A1:F401" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="code"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="type"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="country"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="parent"/>
+    <tableColumn id="6" xr3:uid="{2A55E6B8-C7F9-4E3B-895D-9E5B2B79C42C}" name="Στήλη1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="organizationImage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2087,34 +2091,34 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>257</v>
       </c>
       <c r="D1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E1" t="s">
         <v>256</v>
       </c>
       <c r="F1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G1" t="s">
         <v>254</v>
       </c>
       <c r="H1" t="s">
+        <v>263</v>
+      </c>
+      <c r="I1" t="s">
         <v>264</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>265</v>
-      </c>
-      <c r="J1" t="s">
-        <v>266</v>
       </c>
       <c r="K1" t="s">
         <v>140</v>
@@ -2126,18 +2130,18 @@
         <v>142</v>
       </c>
       <c r="N1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -2176,10 +2180,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -2215,10 +2219,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -2251,10 +2255,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -2287,10 +2291,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -2323,10 +2327,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -2359,10 +2363,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -2395,10 +2399,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -2431,10 +2435,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -2467,10 +2471,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -2503,10 +2507,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -2539,10 +2543,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -2575,10 +2579,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -2611,10 +2615,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -2647,10 +2651,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -2683,10 +2687,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -2695,7 +2699,7 @@
         <v>99</v>
       </c>
       <c r="E17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F17" t="s">
         <v>124</v>
@@ -2719,10 +2723,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -2755,10 +2759,10 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -2791,10 +2795,10 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -2803,7 +2807,7 @@
         <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F20" t="s">
         <v>122</v>
@@ -2827,10 +2831,10 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -2845,7 +2849,7 @@
         <v>124</v>
       </c>
       <c r="G21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K21" t="s">
         <v>187</v>
@@ -2863,10 +2867,10 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -2881,7 +2885,7 @@
         <v>134</v>
       </c>
       <c r="G22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K22" t="s">
         <v>190</v>
@@ -2899,10 +2903,10 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -2917,7 +2921,7 @@
         <v>124</v>
       </c>
       <c r="G23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K23" t="s">
         <v>192</v>
@@ -2935,10 +2939,10 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -2953,7 +2957,7 @@
         <v>122</v>
       </c>
       <c r="G24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K24" t="s">
         <v>195</v>
@@ -2971,10 +2975,10 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -2989,7 +2993,7 @@
         <v>134</v>
       </c>
       <c r="G25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K25" t="s">
         <v>198</v>
@@ -3007,10 +3011,10 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -3025,7 +3029,7 @@
         <v>122</v>
       </c>
       <c r="G26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K26" t="s">
         <v>200</v>
@@ -8946,13 +8950,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D1" t="s">
         <v>59</v>
@@ -8960,7 +8964,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B2" t="s">
         <v>103</v>
@@ -8971,7 +8975,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B3" t="s">
         <v>99</v>
@@ -8982,7 +8986,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B4" t="s">
         <v>103</v>
@@ -9011,7 +9015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScale="252" zoomScaleNormal="252" workbookViewId="0">
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -9034,13 +9038,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C1" t="s">
         <v>263</v>
-      </c>
-      <c r="C1" t="s">
-        <v>264</v>
       </c>
       <c r="D1" t="s">
         <v>254</v>
@@ -9049,13 +9053,13 @@
         <v>257</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G1" t="s">
         <v>205</v>
       </c>
       <c r="H1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I1" t="s">
         <v>206</v>
@@ -9064,7 +9068,7 @@
         <v>207</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L1" t="s">
         <v>208</v>
@@ -9171,16 +9175,16 @@
         <v>210</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D1" t="s">
         <v>59</v>
       </c>
       <c r="E1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" t="s">
         <v>273</v>
-      </c>
-      <c r="F1" t="s">
-        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -9217,16 +9221,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C1" t="s">
         <v>211</v>
       </c>
       <c r="D1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E1" t="s">
         <v>59</v>
@@ -9271,7 +9275,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B1" t="s">
         <v>212</v>
@@ -9283,10 +9287,10 @@
         <v>254</v>
       </c>
       <c r="E1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9294,7 +9298,7 @@
         <v>45936</v>
       </c>
       <c r="C2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
@@ -9311,7 +9315,7 @@
         <v>45937</v>
       </c>
       <c r="C3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D3" t="s">
         <v>68</v>
@@ -9345,7 +9349,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9358,10 +9362,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>249</v>
@@ -9375,7 +9379,7 @@
         <v>213</v>
       </c>
       <c r="B2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C2" t="s">
         <v>214</v>
@@ -9386,10 +9390,10 @@
         <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -9440,13 +9444,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D1" t="s">
         <v>205</v>
@@ -9460,7 +9464,7 @@
         <v>213</v>
       </c>
       <c r="B2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C2" t="str">
         <f>Personnel!$O$2</f>
@@ -9472,10 +9476,10 @@
         <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -9954,7 +9958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -10077,7 +10081,7 @@
         <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C2" t="s">
         <v>68</v>
@@ -10254,7 +10258,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -10271,7 +10275,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -10288,7 +10292,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -10305,7 +10309,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -10395,7 +10399,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B11" t="s">
         <v>202</v>
@@ -10412,7 +10416,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B12" t="s">
         <v>203</v>
@@ -10429,7 +10433,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B13" t="s">
         <v>204</v>
@@ -10446,7 +10450,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B14" t="s">
         <v>202</v>
@@ -10463,7 +10467,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B15" t="s">
         <v>186</v>
@@ -10480,7 +10484,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B16" t="s">
         <v>186</v>
@@ -10497,7 +10501,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B17" t="s">
         <v>194</v>
@@ -10616,7 +10620,7 @@
         <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D2" t="s">
         <v>76</v>
@@ -10637,10 +10641,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10648,9 +10652,11 @@
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>249</v>
       </c>
@@ -10664,10 +10670,13 @@
         <v>254</v>
       </c>
       <c r="E1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+      <c r="F1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -10686,10 +10695,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1001" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>OrganizationType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1001" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E1001" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>NR_CountriesIso2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1001" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>NR_OrgsCode</formula1>
     </dataValidation>
   </dataValidations>
@@ -10760,7 +10769,7 @@
         <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -10777,7 +10786,7 @@
         <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F3" t="s">
         <v>122</v>

</xml_diff>